<commit_message>
[Wordpress Plug-In_User_manual] Plug-In list 작성
</commit_message>
<xml_diff>
--- a/Wordpress Plug-In_User_manual.xlsx
+++ b/Wordpress Plug-In_User_manual.xlsx
@@ -4,28 +4,28 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="7"/>
   </bookViews>
   <sheets>
-    <sheet name="WD-Members" sheetId="4" r:id="rId1"/>
-    <sheet name="Mang Board WP" sheetId="5" r:id="rId2"/>
-    <sheet name="Slider" sheetId="6" r:id="rId3"/>
-    <sheet name="WooCommerce" sheetId="7" r:id="rId4"/>
-    <sheet name="KBoard" sheetId="9" r:id="rId5"/>
-    <sheet name="TinyMCE Advanced" sheetId="10" r:id="rId6"/>
-    <sheet name="Sheet4" sheetId="11" r:id="rId7"/>
-    <sheet name="자이언트 플러그인 list" sheetId="8" r:id="rId8"/>
+    <sheet name="TinyMCE Advanced" sheetId="10" r:id="rId1"/>
+    <sheet name="KBoard" sheetId="9" r:id="rId2"/>
+    <sheet name="WD-Members" sheetId="4" r:id="rId3"/>
+    <sheet name="Mang Board WP" sheetId="5" r:id="rId4"/>
+    <sheet name="Slider" sheetId="6" r:id="rId5"/>
+    <sheet name="WooCommerce" sheetId="7" r:id="rId6"/>
+    <sheet name="자이언트 플러그인 list" sheetId="8" r:id="rId7"/>
+    <sheet name="플러그인 List" sheetId="11" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">Slider!$A$1:$P$94</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'WD-Members'!$A$1:$M$139</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">Slider!$A$1:$P$94</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'WD-Members'!$A$1:$M$139</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="128">
   <si>
     <t>WD-Members widget 추가</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -168,111 +168,183 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>http://giantt.co.kr/6483</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>워드프레스 네이버 신디케이션 연동플러그인 2종</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://giantt.co.kr/7053</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>워드프레스 테마 한글폰트 크기 수정하는 방법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://giantt.co.kr/9383</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한국형 게시판을 만들고 싶다면 Kboard 플러그인추천</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://giantt.co.kr/5443</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kboard 게시판</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>코스모스팜 제작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.cosmosfarm.com/products/kboard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>설치 파일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kboard : 게시판</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kboard comments : 댓글</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플러그인 메뉴에서 플러그인 추가하기를 선택한다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플러그인 추가 화면에서 플러그인 업로드 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파일 선택에서 Download된 zip file를 선택 후 지금 설치하기를 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>설치 방법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 게시판은 워드프레스 페이지로 개설되므로 게시판 생성 메뉴를 사용하기 전에 제목만 적은 페이지를 하나 생성한다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. Kboard 메뉴에서 게시판 생성을 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. 게시판 관리 화면에서 게시판 이름, 게시판이 자동설치될 워드프레스 페이지 등을 설정한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. 게시판 목록에서 생성된 게시판 페이지를 확인한다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시판 생성방법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시판 최신글 뷰 목록 생성 하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Kboard의 최신글 뷰 목록 선택하고 아래와 같이 필요 부분을 설정한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 워드프레스의 기본위젯인 텍스트(임의의 텍스트 또는 HTML) 위젯을 노출하고자 하는 메인화면 위치로 배치한뒤에 (1)번에서 복사해둔 모아보기 숏코드를 입력한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>=&gt; shortcode가 적용되지 않고, text로 인식됨. 원인 파악 필요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TinyMCE Advanced</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Andrew Ozz 제작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>글 또는 페이지의 편집기 플러그인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://giantt.co.kr/5347</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://ko.wordpress.org/plugins/jetpack/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Automattic 제작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">최대 Upload file size가 넘어가므로 WP 플러그인 메뉴에서 설치가 되지 않는다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>압축해제 후 wp-content &gt; plugins 폴더에 copy한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>활성화시 WordPress.com에 연결이 되어야 하기 때문에 Local 가상서버(xampp)에서는 실행이 되지 않는다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>워드프레스 최적화 추천플러그인 WP Clean Up</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>http://giantt.co.kr/6483</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>워드프레스 네이버 신디케이션 연동플러그인 2종</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://giantt.co.kr/7053</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>워드프레스 테마 한글폰트 크기 수정하는 방법</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://giantt.co.kr/9383</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>한국형 게시판을 만들고 싶다면 Kboard 플러그인추천</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://giantt.co.kr/5443</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Kboard 게시판</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>코스모스팜 제작</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://www.cosmosfarm.com/products/kboard</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>설치 파일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>kboard : 게시판</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>kboard comments : 댓글</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>플러그인 메뉴에서 플러그인 추가하기를 선택한다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>플러그인 추가 화면에서 플러그인 업로드 선택한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>파일 선택에서 Download된 zip file를 선택 후 지금 설치하기를 선택한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>설치 방법</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. 게시판은 워드프레스 페이지로 개설되므로 게시판 생성 메뉴를 사용하기 전에 제목만 적은 페이지를 하나 생성한다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2. Kboard 메뉴에서 게시판 생성을 선택한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3. 게시판 관리 화면에서 게시판 이름, 게시판이 자동설치될 워드프레스 페이지 등을 설정한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4. 게시판 목록에서 생성된 게시판 페이지를 확인한다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>게시판 생성방법</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>게시판 최신글 뷰 목록 생성 하기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Kboard의 최신글 뷰 목록 선택하고 아래와 같이 필요 부분을 설정한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2. 워드프레스의 기본위젯인 텍스트(임의의 텍스트 또는 HTML) 위젯을 노출하고자 하는 메인화면 위치로 배치한뒤에 (1)번에서 복사해둔 모아보기 숏코드를 입력한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>=&gt; shortcode가 적용되지 않고, text로 인식됨. 원인 파악 필요</t>
+    <t>https://ko.wordpress.org/plugins/tinymce-advanced/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PlugIn Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Vendor </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CAGE Web Design</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://ko.wordpress.org/plugins/rvg-optimize-database/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Download</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Andrew Ozz</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -280,15 +352,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Andrew Ozz 제작</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://ko.wordpress.org/plugins/tinymce-advanced/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>글 또는 페이지의 편집기 플러그인</t>
+    <t>코스모스팜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한국형 게시판 (댓글 기능 포함)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kboard / kboard comments</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sheet 참조</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -296,31 +372,170 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>http://giantt.co.kr/5347</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://ko.wordpress.org/plugins/jetpack/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사용법</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Automattic 제작</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">최대 Upload file size가 넘어가므로 WP 플러그인 메뉴에서 설치가 되지 않는다. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>압축해제 후 wp-content &gt; plugins 폴더에 copy한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>활성화시 WordPress.com에 연결이 되어야 하기 때문에 Local 가상서버(xampp)에서는 실행이 되지 않는다.</t>
+    <t>JetPack</t>
+  </si>
+  <si>
+    <t>블로그포스트 페이스북,트위터 자동발행</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Automattic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User manual</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://giantt.co.kr/10858</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>revision 및 database 최적화
+스케줄링 기능으로 자동 실행 가능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Optimize Database 
+after Deleting Revisions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사이트를 분석하고 속도를 측정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Google Pagespeed insight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://ko.wordpress.org/plugins/google-pagespeed-insights/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://giantt.co.kr/8786</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Matt Keys</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GZip Ninja Speed Compression</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CustomWPNinjas </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사이트 최적화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>편집기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시판</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Function</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이미지 압축</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://wordpress.org/plugins/gzip-ninja-speed-compression/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://giantt.co.kr/5240</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EWWW Image Optimizer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Shane Bishop </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://wordpress.org/plugins/ewww-image-optimizer/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이미지의 품질은 저하시키지 않으면서 
+불필요한 정보를 제거하여 실질 용량 축소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SNS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스팸댓글차단</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Akismet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Automattic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://ko.wordpress.org/plugins/akismet/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://giantt.co.kr/5118</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">WP Ajax Edit Comments </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://giantt.co.kr/5230</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>워드프레스 댓글 수정및 삭제기능 추가하기
+Akismet과 연동되어 블랙리스트 관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>post date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하마소프트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">네이버 웹마스터도구 플러그인 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.hamasoft.com/hamas-naver-webmaster-tool/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>네이버 웹마스터도구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연동 TOOL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://giantt.co.kr/5381</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -328,7 +543,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -369,6 +584,14 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -378,7 +601,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -386,18 +609,210 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -414,6 +829,231 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="그림 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1219200" y="3848100"/>
+          <a:ext cx="8353425" cy="5876925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="그림 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1266825" y="10401300"/>
+          <a:ext cx="10525125" cy="3752850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="그림 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1257300" y="14782800"/>
+          <a:ext cx="10029825" cy="7581900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="그림 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1304925" y="22888575"/>
+          <a:ext cx="9801225" cy="6572250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1362,7 +2002,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1827,7 +2467,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2885,231 +3525,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="그림 3"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1219200" y="3848100"/>
-          <a:ext cx="8353425" cy="5876925"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="그림 5"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1266825" y="10401300"/>
-          <a:ext cx="10525125" cy="3752850"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>106</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="그림 7"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1257300" y="14782800"/>
-          <a:ext cx="10029825" cy="7581900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>109</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>140</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="그림 9"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1304925" y="22888575"/>
-          <a:ext cx="9801225" cy="6572250"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
@@ -3397,6 +3812,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.375" customWidth="1"/>
+    <col min="2" max="2" width="4.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C4" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D109"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.625" customWidth="1"/>
+    <col min="2" max="2" width="5.5" customWidth="1"/>
+    <col min="3" max="3" width="5.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C4" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D49" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="69" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C69" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="70" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D70" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="108" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D108" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="109" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D109" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D110"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
@@ -3507,7 +4085,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C44"/>
   <sheetViews>
@@ -3563,7 +4141,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E60"/>
   <sheetViews>
@@ -3660,7 +4238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:D8"/>
   <sheetViews>
@@ -3697,188 +4275,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D109"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="3.625" customWidth="1"/>
-    <col min="2" max="2" width="5.5" customWidth="1"/>
-    <col min="3" max="3" width="5.125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C4" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D49" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C69" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="D70" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D108" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D109" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="4.375" customWidth="1"/>
-    <col min="2" max="2" width="4.75" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C4" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3890,82 +4292,82 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C12" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D16" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C18" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -3980,4 +4382,286 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="16.75" style="7" customWidth="1"/>
+    <col min="3" max="3" width="30.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.75" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="59.375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54.375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="H4" s="17">
+        <v>2015.04</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="14"/>
+      <c r="C5" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="H5" s="17">
+        <v>2014.05</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B6" s="14"/>
+      <c r="C6" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6" s="17">
+        <v>2016.03</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="14"/>
+      <c r="C7" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="H7" s="17">
+        <v>2014.05</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B8" s="14"/>
+      <c r="C8" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="H8" s="17">
+        <v>2014.05</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="H9" s="17"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="H10" s="17"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" s="17">
+        <v>2014.06</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="H12" s="24"/>
+    </row>
+    <row r="18" spans="3:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="C18" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="H18" s="6">
+        <v>2014.05</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B4:B8"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F6" r:id="rId1"/>
+    <hyperlink ref="F9" r:id="rId2"/>
+    <hyperlink ref="F10" r:id="rId3"/>
+    <hyperlink ref="F11" r:id="rId4"/>
+    <hyperlink ref="G11" r:id="rId5"/>
+    <hyperlink ref="G6" r:id="rId6"/>
+    <hyperlink ref="F4" r:id="rId7"/>
+    <hyperlink ref="G4" r:id="rId8"/>
+    <hyperlink ref="F7" r:id="rId9"/>
+    <hyperlink ref="G7" r:id="rId10"/>
+    <hyperlink ref="F8" r:id="rId11"/>
+    <hyperlink ref="G8" r:id="rId12"/>
+    <hyperlink ref="F5" r:id="rId13"/>
+    <hyperlink ref="G5" r:id="rId14"/>
+    <hyperlink ref="G18" r:id="rId15"/>
+    <hyperlink ref="F12" r:id="rId16"/>
+    <hyperlink ref="G12" r:id="rId17"/>
+    <hyperlink ref="G9" r:id="rId18"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId19"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[Wordpress Plug-In_User_manual] 테마 list update
</commit_message>
<xml_diff>
--- a/Wordpress Plug-In_User_manual.xlsx
+++ b/Wordpress Plug-In_User_manual.xlsx
@@ -8,27 +8,29 @@
   </bookViews>
   <sheets>
     <sheet name="플러그인 List" sheetId="11" r:id="rId1"/>
-    <sheet name="Akismet" sheetId="12" r:id="rId2"/>
-    <sheet name="KBoard" sheetId="9" r:id="rId3"/>
-    <sheet name="WP-Members" sheetId="4" r:id="rId4"/>
+    <sheet name="테마" sheetId="13" r:id="rId2"/>
+    <sheet name="Akismet" sheetId="12" r:id="rId3"/>
+    <sheet name="KBoard" sheetId="9" r:id="rId4"/>
     <sheet name="Mang Board WP" sheetId="5" r:id="rId5"/>
-    <sheet name="Slider" sheetId="6" r:id="rId6"/>
-    <sheet name="WooCommerce" sheetId="7" r:id="rId7"/>
-    <sheet name="자이언트 플러그인 list" sheetId="8" r:id="rId8"/>
+    <sheet name="WP-Members" sheetId="4" r:id="rId6"/>
+    <sheet name="Slider" sheetId="6" r:id="rId7"/>
+    <sheet name="WooCommerce" sheetId="7" r:id="rId8"/>
+    <sheet name="자이언트 플러그인 list" sheetId="8" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Akismet!$A$1:$Q$221</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">KBoard!$A$1:$Q$130</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">Akismet!$A$1:$Q$221</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">KBoard!$A$1:$Q$130</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'Mang Board WP'!$A$1:$L$87</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="5">Slider!$A$1:$P$80</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'WP-Members'!$A$1:$M$139</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">Slider!$A$1:$P$80</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'WP-Members'!$A$1:$M$139</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">테마!$A$1:$U$63</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="227">
   <si>
     <t>스타일시트 path 설정</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -332,10 +334,6 @@
   </si>
   <si>
     <t>코스모스팜</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>한국형 게시판 (댓글 기능 포함)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -450,10 +448,6 @@
   </si>
   <si>
     <t>SNS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스팸댓글차단</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -751,6 +745,213 @@
   </si>
   <si>
     <t>https://wordpress.org/plugins/wp-members/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plug-In List</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스팸댓글차단
+ - 사업용은 유료 $59</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한국형 게시판 (댓글 기능 포함) - 무료
+겔러리 타입은 스킨 유료 구매해야 함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5 일 ago</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3,000+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.7.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mang Board WP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Hometory </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자료실 게시판, 갤러리(Gallery) 게시판, 캘린더(Calendar) 게시판, 회원관리, 통계관리, 쇼핑몰, 소셜로그인, 소셜공유, 검색엔진최적화(SEO) 등의 다양한 기능을 제공</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>테마 선택시 주요 체크 사항</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 반응형 설계 적용 여부 - Responsive Design</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. Update 지원 여부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 브라우저 호환성 여부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">4. 워드프레스 호환성 문제 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5. SEC 최적화 진원 여부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6. Shortcode 지원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7. 데모 컨텐츠 제공 여부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8. 우커머스 호환지원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>쇼핑몰 기능을 사용하는 경우 반드시 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9. 기타</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>버디프레스, 비비프레스 지원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>언어번역 솔류션</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>슬라이드 옵션</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>추천 테마</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Goodnews</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://giantt.co.kr/8069</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">테마마다 관리자 모드의 사용방법, 숏코드 사용방법, 레이아웃 구성방법등이 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모두 틀리므로 데모컨텐츠(더미파일)은 참고예가 될수 있기 때문입니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>테마</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가격[$]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비주얼컴포저(visual composer)가 기본 제공
+WooCommerce
+BuddyPress
+bbPress</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">AVADA </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Support</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6 monthe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WooCommerce
+BuddyPress
+bbPress
+Gravity Forms
+Digital Downloads
+Easy Digital Downloads
+Events Calendar Pro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://giantt.co.kr/6832</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://demo.theme-fusion.com/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plug-In</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Demo site</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://themes.momizat.com/themes.php?theme=goodnews</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sales</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Created</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Last Update</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Newspaper </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  5 April 17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  21 February 17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://demo.tagdiv.com/select_demo/select_demo_newspaper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://forum.tagdiv.com/newspaper-theme-documentation/</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -828,12 +1029,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="15">
@@ -1052,7 +1259,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -1113,9 +1320,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1131,6 +1335,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1143,7 +1348,81 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="쉼표 [0]" xfId="2" builtinId="6"/>
@@ -1164,6 +1443,66 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>447261</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>91110</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>516156</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>99393</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="그림 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5922065" y="505240"/>
+          <a:ext cx="2984374" cy="4356653"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2691,7 +3030,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2977,7 +3316,472 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="그룹 1"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="981075" y="885825"/>
+          <a:ext cx="1666875" cy="2657475"/>
+          <a:chOff x="1323975" y="885825"/>
+          <a:chExt cx="1666875" cy="2657475"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="3" name="그림 2"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1323975" y="885825"/>
+            <a:ext cx="1666875" cy="2657475"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="모서리가 둥근 직사각형 3"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1333500" y="1609725"/>
+            <a:ext cx="1419225" cy="323850"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="5" name="그룹 4"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="714375" y="4038599"/>
+          <a:ext cx="6248400" cy="2600325"/>
+          <a:chOff x="1257300" y="3981450"/>
+          <a:chExt cx="9515475" cy="3333750"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="6" name="그림 5"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1257300" y="3981450"/>
+            <a:ext cx="9515475" cy="3333750"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="모서리가 둥근 직사각형 6"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1390650" y="4238624"/>
+            <a:ext cx="7496175" cy="542925"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="8" name="그룹 7"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="771525" y="6981825"/>
+          <a:ext cx="6076950" cy="1905000"/>
+          <a:chOff x="1257300" y="7753350"/>
+          <a:chExt cx="7991475" cy="2095500"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="9" name="그림 8"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1257300" y="7753350"/>
+            <a:ext cx="7991475" cy="2095500"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="모서리가 둥근 직사각형 9"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1600200" y="8886825"/>
+            <a:ext cx="2505075" cy="200026"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="11" name="그룹 10"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="771525" y="9258301"/>
+          <a:ext cx="5524500" cy="3162300"/>
+          <a:chOff x="1257300" y="10058400"/>
+          <a:chExt cx="5772150" cy="3457575"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="12" name="그림 11"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1257300" y="10058400"/>
+            <a:ext cx="5772150" cy="3457575"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="13" name="모서리가 둥근 직사각형 12"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1381125" y="12706349"/>
+            <a:ext cx="2562225" cy="276225"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3926,472 +4730,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="2" name="그룹 1"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="981075" y="885825"/>
-          <a:ext cx="1666875" cy="2657475"/>
-          <a:chOff x="1323975" y="885825"/>
-          <a:chExt cx="1666875" cy="2657475"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="3" name="그림 2"/>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-            <a:extLst>
-              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-              </a:ext>
-            </a:extLst>
-          </a:blip>
-          <a:srcRect/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="1323975" y="885825"/>
-            <a:ext cx="1666875" cy="2657475"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:extLst>
-            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a14:hiddenFill>
-            </a:ext>
-          </a:extLst>
-        </xdr:spPr>
-      </xdr:pic>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="4" name="모서리가 둥근 직사각형 3"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1333500" y="1609725"/>
-            <a:ext cx="1419225" cy="323850"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFF00"/>
-            </a:solidFill>
-            <a:prstDash val="sysDash"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="5" name="그룹 4"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="714375" y="4038599"/>
-          <a:ext cx="6248400" cy="2600325"/>
-          <a:chOff x="1257300" y="3981450"/>
-          <a:chExt cx="9515475" cy="3333750"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="6" name="그림 5"/>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-            <a:extLst>
-              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-              </a:ext>
-            </a:extLst>
-          </a:blip>
-          <a:srcRect/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="1257300" y="3981450"/>
-            <a:ext cx="9515475" cy="3333750"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:extLst>
-            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a14:hiddenFill>
-            </a:ext>
-          </a:extLst>
-        </xdr:spPr>
-      </xdr:pic>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="7" name="모서리가 둥근 직사각형 6"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1390650" y="4238624"/>
-            <a:ext cx="7496175" cy="542925"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-            <a:prstDash val="sysDash"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="8" name="그룹 7"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="771525" y="6981825"/>
-          <a:ext cx="6076950" cy="1905000"/>
-          <a:chOff x="1257300" y="7753350"/>
-          <a:chExt cx="7991475" cy="2095500"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="9" name="그림 8"/>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-            <a:extLst>
-              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-              </a:ext>
-            </a:extLst>
-          </a:blip>
-          <a:srcRect/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="1257300" y="7753350"/>
-            <a:ext cx="7991475" cy="2095500"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:extLst>
-            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a14:hiddenFill>
-            </a:ext>
-          </a:extLst>
-        </xdr:spPr>
-      </xdr:pic>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="10" name="모서리가 둥근 직사각형 9"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1600200" y="8886825"/>
-            <a:ext cx="2505075" cy="200026"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-            <a:prstDash val="sysDash"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>57151</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="11" name="그룹 10"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="771525" y="9258301"/>
-          <a:ext cx="5524500" cy="3162300"/>
-          <a:chOff x="1257300" y="10058400"/>
-          <a:chExt cx="5772150" cy="3457575"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="12" name="그림 11"/>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-            <a:extLst>
-              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-              </a:ext>
-            </a:extLst>
-          </a:blip>
-          <a:srcRect/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="1257300" y="10058400"/>
-            <a:ext cx="5772150" cy="3457575"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:extLst>
-            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a14:hiddenFill>
-            </a:ext>
-          </a:extLst>
-        </xdr:spPr>
-      </xdr:pic>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="13" name="모서리가 둥근 직사각형 12"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1381125" y="12706349"/>
-            <a:ext cx="2562225" cy="276225"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-            <a:prstDash val="sysDash"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5704,10 +6043,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K23"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5719,17 +6058,22 @@
     <col min="5" max="5" width="37.75" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.625" style="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.375" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="70.375" style="6" customWidth="1"/>
+    <col min="8" max="8" width="8.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="54.25" style="6" customWidth="1"/>
     <col min="10" max="10" width="23.25" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.125" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B1" s="34" t="s">
+        <v>178</v>
+      </c>
+    </row>
     <row r="2" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:11" s="8" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>69</v>
@@ -5741,69 +6085,69 @@
         <v>74</v>
       </c>
       <c r="F3" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="G3" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="G3" s="19" t="s">
-        <v>126</v>
-      </c>
       <c r="H3" s="19" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I3" s="19" t="s">
         <v>73</v>
       </c>
       <c r="J3" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K3" s="20" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="24"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="22" t="s">
+      <c r="J4" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="J4" s="22" t="s">
-        <v>90</v>
       </c>
       <c r="K4" s="23">
         <v>2015.04</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" ht="33" x14ac:dyDescent="0.3">
       <c r="B5" s="31"/>
-      <c r="C5" s="9" t="s">
-        <v>151</v>
+      <c r="C5" s="35" t="s">
+        <v>149</v>
       </c>
       <c r="D5" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="F5" s="25"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="J5" s="10" t="s">
         <v>108</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>110</v>
       </c>
       <c r="K5" s="11">
         <v>2014.05</v>
@@ -5812,22 +6156,22 @@
     <row r="6" spans="2:11" ht="33" x14ac:dyDescent="0.3">
       <c r="B6" s="31"/>
       <c r="C6" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>71</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="F6" s="27"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+        <v>84</v>
+      </c>
+      <c r="F6" s="26"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="26"/>
       <c r="I6" s="10" t="s">
         <v>72</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K6" s="11">
         <v>2016.03</v>
@@ -5836,22 +6180,22 @@
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="31"/>
       <c r="C7" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>93</v>
-      </c>
       <c r="E7" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" s="25"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="10" t="s">
+      <c r="J7" s="10" t="s">
         <v>99</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>100</v>
       </c>
       <c r="K7" s="11">
         <v>2014.05</v>
@@ -5860,22 +6204,22 @@
     <row r="8" spans="2:11" ht="33" x14ac:dyDescent="0.3">
       <c r="B8" s="31"/>
       <c r="C8" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="E8" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="F8" s="26"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="F8" s="27"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="10" t="s">
-        <v>103</v>
-      </c>
       <c r="J8" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K8" s="11">
         <v>2014.05</v>
@@ -5883,10 +6227,10 @@
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>147</v>
+        <v>94</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>145</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>75</v>
@@ -5894,220 +6238,232 @@
       <c r="E9" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="F9" s="26"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="25"/>
       <c r="I9" s="10" t="s">
         <v>68</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K9" s="11"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B10" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="C10" s="14" t="s">
+    <row r="10" spans="2:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="B10" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>184</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G10" s="38" t="s">
+        <v>182</v>
+      </c>
+      <c r="H10" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="I10" s="10"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="11"/>
+    </row>
+    <row r="11" spans="2:11" ht="33" x14ac:dyDescent="0.3">
+      <c r="B11" s="33"/>
+      <c r="C11" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="F11" s="25"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="F10" s="26"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="K10" s="11"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="C11" s="14" t="s">
+      <c r="K11" s="11"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="E12" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="F12" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="G12" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="H12" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="I12" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="H11" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="K11" s="11"/>
-    </row>
-    <row r="12" spans="2:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="B12" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="C12" s="9" t="s">
+      <c r="J12" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="K12" s="11"/>
+    </row>
+    <row r="13" spans="2:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="B13" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D12" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="F12" s="26" t="s">
+      <c r="E13" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="I12" s="10" t="s">
+      <c r="F13" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="G13" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="H13" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="I13" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="J13" s="10" t="s">
         <v>60</v>
-      </c>
-      <c r="K12" s="11">
-        <v>2014.06</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B13" s="33"/>
-      <c r="C13" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="F13" s="26" t="s">
-        <v>139</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="J13" s="10" t="s">
-        <v>142</v>
       </c>
       <c r="K13" s="11">
         <v>2014.06</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="32" t="s">
-        <v>127</v>
-      </c>
+    <row r="14" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B14" s="33"/>
       <c r="C14" s="9" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="F14" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="G14" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="H14" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="K14" s="11">
+        <v>2014.06</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B15" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="G14" s="24">
-        <v>6000</v>
-      </c>
-      <c r="H14" s="24"/>
-      <c r="I14" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="J14" s="9"/>
-      <c r="K14" s="11"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="33"/>
       <c r="C15" s="9" t="s">
         <v>117</v>
       </c>
       <c r="D15" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="F15" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="G15" s="40">
+        <v>6000</v>
+      </c>
+      <c r="H15" s="42"/>
+      <c r="I15" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="J15" s="9"/>
+      <c r="K15" s="11"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B16" s="33"/>
+      <c r="C16" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="F16" s="26"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="K16" s="11">
+        <v>2014.06</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="F15" s="27"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="J15" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="K15" s="11">
-        <v>2014.06</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="C16" s="9" t="s">
+      <c r="E17" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="F17" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="G17" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="H17" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="I17" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="F16" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="J16" s="9"/>
-      <c r="K16" s="11"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B17" s="13"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="11"/>
     </row>
@@ -6116,53 +6472,53 @@
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="25"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
       <c r="K18" s="11"/>
     </row>
-    <row r="19" spans="2:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" s="13"/>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="11"/>
+    </row>
+    <row r="20" spans="2:11" ht="33" x14ac:dyDescent="0.3">
+      <c r="B20" s="13"/>
+      <c r="C20" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="F19" s="27"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="K19" s="11">
+      <c r="F20" s="26"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="K20" s="11">
         <v>2014.05</v>
       </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B20" s="13"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="11"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" s="13"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="25"/>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
       <c r="K21" s="11"/>
@@ -6172,38 +6528,51 @@
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="25"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
       <c r="K22" s="11"/>
     </row>
-    <row r="23" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="15"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="17"/>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B23" s="13"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="11"/>
+    </row>
+    <row r="24" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="15"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B4:B8"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B10:B11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I6" r:id="rId1"/>
     <hyperlink ref="I9" r:id="rId2"/>
-    <hyperlink ref="I10" r:id="rId3"/>
-    <hyperlink ref="I12" r:id="rId4"/>
-    <hyperlink ref="J12" r:id="rId5"/>
+    <hyperlink ref="I11" r:id="rId3"/>
+    <hyperlink ref="I13" r:id="rId4"/>
+    <hyperlink ref="J13" r:id="rId5"/>
     <hyperlink ref="J6" r:id="rId6"/>
     <hyperlink ref="I4" r:id="rId7"/>
     <hyperlink ref="J4" r:id="rId8"/>
@@ -6213,15 +6582,15 @@
     <hyperlink ref="J8" r:id="rId12"/>
     <hyperlink ref="I5" r:id="rId13"/>
     <hyperlink ref="J5" r:id="rId14"/>
-    <hyperlink ref="J19" r:id="rId15"/>
+    <hyperlink ref="J20" r:id="rId15"/>
     <hyperlink ref="J9" r:id="rId16"/>
-    <hyperlink ref="I15" r:id="rId17"/>
-    <hyperlink ref="J15" r:id="rId18"/>
-    <hyperlink ref="I14" r:id="rId19"/>
-    <hyperlink ref="I16" r:id="rId20"/>
-    <hyperlink ref="I13" r:id="rId21"/>
-    <hyperlink ref="J13" r:id="rId22"/>
-    <hyperlink ref="I11" r:id="rId23"/>
+    <hyperlink ref="I16" r:id="rId17"/>
+    <hyperlink ref="J16" r:id="rId18"/>
+    <hyperlink ref="I15" r:id="rId19"/>
+    <hyperlink ref="I17" r:id="rId20"/>
+    <hyperlink ref="I14" r:id="rId21"/>
+    <hyperlink ref="J14" r:id="rId22"/>
+    <hyperlink ref="I12" r:id="rId23"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId24"/>
@@ -6230,9 +6599,354 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:K37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A19" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="3.125" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="38.25" customWidth="1"/>
+    <col min="10" max="10" width="22.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C25" s="44" t="s">
+        <v>206</v>
+      </c>
+      <c r="D25" s="45" t="s">
+        <v>220</v>
+      </c>
+      <c r="E25" s="45" t="s">
+        <v>221</v>
+      </c>
+      <c r="F25" s="45" t="s">
+        <v>207</v>
+      </c>
+      <c r="G25" s="45" t="s">
+        <v>219</v>
+      </c>
+      <c r="H25" s="45" t="s">
+        <v>210</v>
+      </c>
+      <c r="I25" s="45" t="s">
+        <v>215</v>
+      </c>
+      <c r="J25" s="45" t="s">
+        <v>216</v>
+      </c>
+      <c r="K25" s="46" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="C26" s="57" t="s">
+        <v>209</v>
+      </c>
+      <c r="D26" s="47">
+        <v>41137</v>
+      </c>
+      <c r="E26" s="48" t="s">
+        <v>223</v>
+      </c>
+      <c r="F26" s="12">
+        <v>60</v>
+      </c>
+      <c r="G26" s="49">
+        <v>312924</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="J26" s="50" t="s">
+        <v>213</v>
+      </c>
+      <c r="K26" s="51" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="C27" s="57" t="s">
+        <v>222</v>
+      </c>
+      <c r="D27" s="47">
+        <v>41521</v>
+      </c>
+      <c r="E27" s="48">
+        <v>42835</v>
+      </c>
+      <c r="F27" s="12">
+        <v>59</v>
+      </c>
+      <c r="G27" s="49">
+        <v>39881</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="I27" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="J27" s="50" t="s">
+        <v>226</v>
+      </c>
+      <c r="K27" s="51" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" ht="66.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C28" s="58" t="s">
+        <v>202</v>
+      </c>
+      <c r="D28" s="52">
+        <v>40900</v>
+      </c>
+      <c r="E28" s="53" t="s">
+        <v>224</v>
+      </c>
+      <c r="F28" s="43">
+        <v>64</v>
+      </c>
+      <c r="G28" s="54">
+        <v>6741</v>
+      </c>
+      <c r="H28" s="43" t="s">
+        <v>211</v>
+      </c>
+      <c r="I28" s="43" t="s">
+        <v>208</v>
+      </c>
+      <c r="J28" s="55" t="s">
+        <v>203</v>
+      </c>
+      <c r="K28" s="56" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+    </row>
+    <row r="33" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+    </row>
+    <row r="34" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+    </row>
+    <row r="35" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+    </row>
+    <row r="36" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+    </row>
+    <row r="37" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="J28" r:id="rId1"/>
+    <hyperlink ref="J26" r:id="rId2"/>
+    <hyperlink ref="K26" r:id="rId3"/>
+    <hyperlink ref="K28" r:id="rId4"/>
+    <hyperlink ref="K27" r:id="rId5"/>
+    <hyperlink ref="J27" r:id="rId6"/>
+  </hyperlinks>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="56" orientation="portrait" r:id="rId7"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="11" max="62" man="1"/>
+  </colBreaks>
+  <ignoredErrors>
+    <ignoredError sqref="E26" twoDigitTextYear="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId8"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E200"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A148" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A64" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="T163" sqref="T163"/>
     </sheetView>
   </sheetViews>
@@ -6245,97 +6959,97 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C3" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C4" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C6" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="41" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D41" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="58" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D58" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="76" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D76" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="77" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E77" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="78" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E78" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="97" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D97" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="115" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D115" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="129" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D129" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="144" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D144" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="165" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D165" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="166" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E166" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="192" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E192" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="200" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D200" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -6349,12 +7063,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D102"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="Q108" sqref="Q108"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A67" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6374,7 +7088,7 @@
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="29" t="s">
         <v>44</v>
       </c>
     </row>
@@ -6450,17 +7164,17 @@
     </row>
     <row r="100" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D100" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="101" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D101" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="102" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D102" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -6474,7 +7188,63 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C44"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.125" customWidth="1"/>
+    <col min="2" max="2" width="4.5" style="4" customWidth="1"/>
+    <col min="3" max="3" width="4.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="98" orientation="portrait" r:id="rId1"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="43" max="16383" man="1"/>
+  </rowBreaks>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D110"/>
   <sheetViews>
@@ -6491,7 +7261,7 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
@@ -6501,7 +7271,7 @@
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C4" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
@@ -6586,63 +7356,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C44"/>
-  <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="P51" sqref="P51"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="3.125" customWidth="1"/>
-    <col min="2" max="2" width="4.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="4.375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C33" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C44" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="98" orientation="portrait" r:id="rId1"/>
-  <rowBreaks count="1" manualBreakCount="1">
-    <brk id="43" max="16383" man="1"/>
-  </rowBreaks>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E58"/>
   <sheetViews>
@@ -6742,7 +7456,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:D8"/>
   <sheetViews>
@@ -6779,7 +7493,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D23"/>
   <sheetViews>
@@ -6836,7 +7550,7 @@
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
[Avada] initial upload data
</commit_message>
<xml_diff>
--- a/Wordpress Plug-In_User_manual.xlsx
+++ b/Wordpress Plug-In_User_manual.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -1336,18 +1336,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1422,6 +1410,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -5799,7 +5799,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5834,7 +5834,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6066,7 +6066,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="30" t="s">
         <v>178</v>
       </c>
     </row>
@@ -6104,7 +6104,7 @@
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="55" t="s">
         <v>93</v>
       </c>
       <c r="C4" s="21" t="s">
@@ -6117,7 +6117,7 @@
         <v>86</v>
       </c>
       <c r="F4" s="24"/>
-      <c r="G4" s="37"/>
+      <c r="G4" s="33"/>
       <c r="H4" s="24"/>
       <c r="I4" s="22" t="s">
         <v>88</v>
@@ -6130,8 +6130,8 @@
       </c>
     </row>
     <row r="5" spans="2:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="B5" s="31"/>
-      <c r="C5" s="35" t="s">
+      <c r="B5" s="56"/>
+      <c r="C5" s="31" t="s">
         <v>149</v>
       </c>
       <c r="D5" s="9" t="s">
@@ -6141,7 +6141,7 @@
         <v>179</v>
       </c>
       <c r="F5" s="25"/>
-      <c r="G5" s="38"/>
+      <c r="G5" s="34"/>
       <c r="H5" s="25"/>
       <c r="I5" s="10" t="s">
         <v>107</v>
@@ -6154,7 +6154,7 @@
       </c>
     </row>
     <row r="6" spans="2:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="B6" s="31"/>
+      <c r="B6" s="56"/>
       <c r="C6" s="12" t="s">
         <v>85</v>
       </c>
@@ -6165,7 +6165,7 @@
         <v>84</v>
       </c>
       <c r="F6" s="26"/>
-      <c r="G6" s="39"/>
+      <c r="G6" s="35"/>
       <c r="H6" s="26"/>
       <c r="I6" s="10" t="s">
         <v>72</v>
@@ -6178,7 +6178,7 @@
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="31"/>
+      <c r="B7" s="56"/>
       <c r="C7" s="9" t="s">
         <v>91</v>
       </c>
@@ -6189,7 +6189,7 @@
         <v>97</v>
       </c>
       <c r="F7" s="25"/>
-      <c r="G7" s="38"/>
+      <c r="G7" s="34"/>
       <c r="H7" s="25"/>
       <c r="I7" s="10" t="s">
         <v>98</v>
@@ -6202,7 +6202,7 @@
       </c>
     </row>
     <row r="8" spans="2:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="B8" s="31"/>
+      <c r="B8" s="56"/>
       <c r="C8" s="9" t="s">
         <v>100</v>
       </c>
@@ -6213,7 +6213,7 @@
         <v>103</v>
       </c>
       <c r="F8" s="26"/>
-      <c r="G8" s="39"/>
+      <c r="G8" s="35"/>
       <c r="H8" s="26"/>
       <c r="I8" s="10" t="s">
         <v>102</v>
@@ -6229,7 +6229,7 @@
       <c r="B9" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="32" t="s">
         <v>145</v>
       </c>
       <c r="D9" s="9" t="s">
@@ -6239,7 +6239,7 @@
         <v>59</v>
       </c>
       <c r="F9" s="25"/>
-      <c r="G9" s="38"/>
+      <c r="G9" s="34"/>
       <c r="H9" s="25"/>
       <c r="I9" s="10" t="s">
         <v>68</v>
@@ -6250,10 +6250,10 @@
       <c r="K9" s="11"/>
     </row>
     <row r="10" spans="2:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="32" t="s">
         <v>184</v>
       </c>
       <c r="D10" s="9" t="s">
@@ -6265,7 +6265,7 @@
       <c r="F10" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="G10" s="38" t="s">
+      <c r="G10" s="34" t="s">
         <v>182</v>
       </c>
       <c r="H10" s="25" t="s">
@@ -6276,8 +6276,8 @@
       <c r="K10" s="11"/>
     </row>
     <row r="11" spans="2:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="B11" s="33"/>
-      <c r="C11" s="36" t="s">
+      <c r="B11" s="58"/>
+      <c r="C11" s="32" t="s">
         <v>77</v>
       </c>
       <c r="D11" s="9" t="s">
@@ -6287,7 +6287,7 @@
         <v>180</v>
       </c>
       <c r="F11" s="25"/>
-      <c r="G11" s="38"/>
+      <c r="G11" s="34"/>
       <c r="H11" s="25"/>
       <c r="I11" s="10" t="s">
         <v>44</v>
@@ -6313,7 +6313,7 @@
       <c r="F12" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="34" t="s">
         <v>175</v>
       </c>
       <c r="H12" s="25" t="s">
@@ -6328,7 +6328,7 @@
       <c r="K12" s="11"/>
     </row>
     <row r="13" spans="2:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="57" t="s">
         <v>104</v>
       </c>
       <c r="C13" s="9" t="s">
@@ -6343,7 +6343,7 @@
       <c r="F13" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="G13" s="38" t="s">
+      <c r="G13" s="34" t="s">
         <v>130</v>
       </c>
       <c r="H13" s="25" t="s">
@@ -6360,7 +6360,7 @@
       </c>
     </row>
     <row r="14" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B14" s="33"/>
+      <c r="B14" s="58"/>
       <c r="C14" s="9" t="s">
         <v>136</v>
       </c>
@@ -6373,7 +6373,7 @@
       <c r="F14" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="G14" s="38" t="s">
+      <c r="G14" s="34" t="s">
         <v>138</v>
       </c>
       <c r="H14" s="25" t="s">
@@ -6390,7 +6390,7 @@
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="57" t="s">
         <v>125</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -6405,10 +6405,10 @@
       <c r="F15" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="G15" s="40">
+      <c r="G15" s="36">
         <v>6000</v>
       </c>
-      <c r="H15" s="42"/>
+      <c r="H15" s="38"/>
       <c r="I15" s="10" t="s">
         <v>120</v>
       </c>
@@ -6416,7 +6416,7 @@
       <c r="K15" s="11"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="33"/>
+      <c r="B16" s="58"/>
       <c r="C16" s="9" t="s">
         <v>115</v>
       </c>
@@ -6427,7 +6427,7 @@
         <v>126</v>
       </c>
       <c r="F16" s="26"/>
-      <c r="G16" s="39"/>
+      <c r="G16" s="35"/>
       <c r="H16" s="26"/>
       <c r="I16" s="10" t="s">
         <v>114</v>
@@ -6455,7 +6455,7 @@
       <c r="F17" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="G17" s="38" t="s">
+      <c r="G17" s="34" t="s">
         <v>130</v>
       </c>
       <c r="H17" s="25" t="s">
@@ -6473,7 +6473,7 @@
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="F18" s="25"/>
-      <c r="G18" s="38"/>
+      <c r="G18" s="34"/>
       <c r="H18" s="25"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
@@ -6485,7 +6485,7 @@
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
       <c r="F19" s="25"/>
-      <c r="G19" s="38"/>
+      <c r="G19" s="34"/>
       <c r="H19" s="25"/>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
@@ -6501,7 +6501,7 @@
         <v>111</v>
       </c>
       <c r="F20" s="26"/>
-      <c r="G20" s="39"/>
+      <c r="G20" s="35"/>
       <c r="H20" s="26"/>
       <c r="I20" s="9"/>
       <c r="J20" s="10" t="s">
@@ -6517,7 +6517,7 @@
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="25"/>
-      <c r="G21" s="38"/>
+      <c r="G21" s="34"/>
       <c r="H21" s="25"/>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
@@ -6529,7 +6529,7 @@
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
       <c r="F22" s="25"/>
-      <c r="G22" s="38"/>
+      <c r="G22" s="34"/>
       <c r="H22" s="25"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -6541,7 +6541,7 @@
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="25"/>
-      <c r="G23" s="38"/>
+      <c r="G23" s="34"/>
       <c r="H23" s="25"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -6553,7 +6553,7 @@
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
       <c r="F24" s="27"/>
-      <c r="G24" s="41"/>
+      <c r="G24" s="37"/>
       <c r="H24" s="27"/>
       <c r="I24" s="16"/>
       <c r="J24" s="16"/>
@@ -6602,7 +6602,7 @@
   <dimension ref="A3:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A19" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6706,48 +6706,48 @@
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C25" s="44" t="s">
+      <c r="C25" s="40" t="s">
         <v>206</v>
       </c>
-      <c r="D25" s="45" t="s">
+      <c r="D25" s="41" t="s">
         <v>220</v>
       </c>
-      <c r="E25" s="45" t="s">
+      <c r="E25" s="41" t="s">
         <v>221</v>
       </c>
-      <c r="F25" s="45" t="s">
+      <c r="F25" s="41" t="s">
         <v>207</v>
       </c>
-      <c r="G25" s="45" t="s">
+      <c r="G25" s="41" t="s">
         <v>219</v>
       </c>
-      <c r="H25" s="45" t="s">
+      <c r="H25" s="41" t="s">
         <v>210</v>
       </c>
-      <c r="I25" s="45" t="s">
+      <c r="I25" s="41" t="s">
         <v>215</v>
       </c>
-      <c r="J25" s="45" t="s">
+      <c r="J25" s="41" t="s">
         <v>216</v>
       </c>
-      <c r="K25" s="46" t="s">
+      <c r="K25" s="42" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="26" spans="2:11" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="C26" s="57" t="s">
+      <c r="C26" s="53" t="s">
         <v>209</v>
       </c>
-      <c r="D26" s="47">
+      <c r="D26" s="43">
         <v>41137</v>
       </c>
-      <c r="E26" s="48" t="s">
+      <c r="E26" s="44" t="s">
         <v>223</v>
       </c>
       <c r="F26" s="12">
         <v>60</v>
       </c>
-      <c r="G26" s="49">
+      <c r="G26" s="45">
         <v>312924</v>
       </c>
       <c r="H26" s="12" t="s">
@@ -6756,27 +6756,27 @@
       <c r="I26" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="J26" s="50" t="s">
+      <c r="J26" s="46" t="s">
         <v>213</v>
       </c>
-      <c r="K26" s="51" t="s">
+      <c r="K26" s="47" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="27" spans="2:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="C27" s="57" t="s">
+      <c r="C27" s="53" t="s">
         <v>222</v>
       </c>
-      <c r="D27" s="47">
+      <c r="D27" s="43">
         <v>41521</v>
       </c>
-      <c r="E27" s="48">
+      <c r="E27" s="44">
         <v>42835</v>
       </c>
       <c r="F27" s="12">
         <v>59</v>
       </c>
-      <c r="G27" s="49">
+      <c r="G27" s="45">
         <v>39881</v>
       </c>
       <c r="H27" s="12" t="s">
@@ -6785,39 +6785,39 @@
       <c r="I27" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="J27" s="50" t="s">
+      <c r="J27" s="46" t="s">
         <v>226</v>
       </c>
-      <c r="K27" s="51" t="s">
+      <c r="K27" s="47" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="28" spans="2:11" ht="66.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C28" s="58" t="s">
+      <c r="C28" s="54" t="s">
         <v>202</v>
       </c>
-      <c r="D28" s="52">
+      <c r="D28" s="48">
         <v>40900</v>
       </c>
-      <c r="E28" s="53" t="s">
+      <c r="E28" s="49" t="s">
         <v>224</v>
       </c>
-      <c r="F28" s="43">
+      <c r="F28" s="39">
         <v>64</v>
       </c>
-      <c r="G28" s="54">
+      <c r="G28" s="50">
         <v>6741</v>
       </c>
-      <c r="H28" s="43" t="s">
+      <c r="H28" s="39" t="s">
         <v>211</v>
       </c>
-      <c r="I28" s="43" t="s">
+      <c r="I28" s="39" t="s">
         <v>208</v>
       </c>
-      <c r="J28" s="55" t="s">
+      <c r="J28" s="51" t="s">
         <v>203</v>
       </c>
-      <c r="K28" s="56" t="s">
+      <c r="K28" s="52" t="s">
         <v>218</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Wordpress Plug-In_User_manual] Loco Translate 추가
</commit_message>
<xml_diff>
--- a/Wordpress Plug-In_User_manual.xlsx
+++ b/Wordpress Plug-In_User_manual.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="플러그인 List" sheetId="11" r:id="rId1"/>
@@ -25,12 +25,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="5">'WP-Members'!$A$1:$M$139</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">테마!$A$1:$U$63</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="237">
   <si>
     <t>스타일시트 path 설정</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -952,6 +952,46 @@
   </si>
   <si>
     <t>http://forum.tagdiv.com/newspaper-theme-documentation/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한글파일 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Loco Translate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tim Whitlock</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>themes나 plugin의 번역 파일 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>400,000+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 개월 전에</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.7.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://wordpress.org/plugins/loco-translate/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://docs.woocommerce.com/document/woocommerce-localization/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017.07.25</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -6045,8 +6085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6512,16 +6552,36 @@
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B21" s="13"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="11"/>
+      <c r="B21" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="G21" s="34" t="s">
+        <v>231</v>
+      </c>
+      <c r="H21" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="K21" s="11" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" s="13"/>
@@ -6591,9 +6651,11 @@
     <hyperlink ref="I14" r:id="rId21"/>
     <hyperlink ref="J14" r:id="rId22"/>
     <hyperlink ref="I12" r:id="rId23"/>
+    <hyperlink ref="I21" r:id="rId24"/>
+    <hyperlink ref="J21" r:id="rId25"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId24"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId26"/>
 </worksheet>
 </file>
 
@@ -6601,7 +6663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A19" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A19" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[Wordpress Plug-In_User_manual] woocommerce 관련 plug in 추가 - 추가 update 필요
</commit_message>
<xml_diff>
--- a/Wordpress Plug-In_User_manual.xlsx
+++ b/Wordpress Plug-In_User_manual.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="239">
   <si>
     <t>스타일시트 path 설정</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -992,6 +992,14 @@
   </si>
   <si>
     <t>2017.07.25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우커머스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인/회원 가입 시 이동할 페이지 지정하기</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5839,7 +5847,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5874,7 +5882,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6086,7 +6094,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6584,10 +6592,14 @@
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B22" s="13"/>
+      <c r="B22" s="13" t="s">
+        <v>237</v>
+      </c>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
+      <c r="E22" s="9" t="s">
+        <v>238</v>
+      </c>
       <c r="F22" s="25"/>
       <c r="G22" s="34"/>
       <c r="H22" s="25"/>

</xml_diff>